<commit_message>
added examination rule sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/Bewertungsbogen.xlsx
+++ b/src/main/resources/Bewertungsbogen.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Madleen\Desktop\W O R K\Studium\Semester 2\SE2\organizing-tool\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freyh\Nextcloud\HdM\SS20 - Semester 2\Software Entwichlung 2 (113215a)\organizing-tool\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCF311C-7F98-4A36-933E-A632889BBA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="3330" yWindow="2280" windowWidth="28010" windowHeight="15860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt" sheetId="1" r:id="rId1"/>
@@ -17,8 +18,16 @@
     <sheet name="Gesamtnote" sheetId="3" r:id="rId3"/>
     <sheet name="Notenspiegel" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -27,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -148,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -206,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -263,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -292,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -527,7 +536,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -628,8 +637,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Erklärender Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,7 +670,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1044" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1044" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -704,7 +719,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1042" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1042" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -747,7 +768,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1040" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1040" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -790,7 +817,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1038" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1038" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -833,7 +866,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1036" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1036" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -876,7 +915,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1034" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1034" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -919,7 +964,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1032" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1032" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -962,7 +1013,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1005,7 +1062,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1048,7 +1111,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1096,7 +1165,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1449,36 +1524,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="8.26953125" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" customWidth="1"/>
-    <col min="20" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" customWidth="1"/>
+    <col min="16" max="16" width="8.54296875" customWidth="1"/>
+    <col min="17" max="17" width="20.7265625" customWidth="1"/>
+    <col min="18" max="18" width="22.453125" customWidth="1"/>
+    <col min="19" max="19" width="23.7265625" customWidth="1"/>
+    <col min="20" max="1025" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>56</v>
       </c>
@@ -1592,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>60</v>
       </c>
@@ -1608,16 +1683,46 @@
       <c r="F3" t="s">
         <v>59</v>
       </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
       <c r="Q3" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="S3" s="3">
         <f>VLOOKUP(Q3,Notenspiegel!$D$17:$E$47,2,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>63</v>
       </c>
@@ -1642,7 +1747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q5" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1652,7 +1757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q6" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1662,7 +1767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1672,7 +1777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1682,7 +1787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1692,7 +1797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1702,7 +1807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1712,7 +1817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1722,7 +1827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1732,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1742,7 +1847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1752,7 +1857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="Q16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1762,7 +1867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q17" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1772,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q18" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1782,7 +1887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1792,7 +1897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1802,7 +1907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1812,7 +1917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1822,7 +1927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1832,7 +1937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1842,7 +1947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1852,7 +1957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1862,7 +1967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q27" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1872,7 +1977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1882,7 +1987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q29" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1892,7 +1997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q30" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1902,7 +2007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q31" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1912,7 +2017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q32" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1922,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q33" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1932,7 +2037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q34" s="3">
         <f t="shared" ref="Q34:Q65" si="1">SUM(G34:P34)</f>
         <v>0</v>
@@ -1942,7 +2047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1952,7 +2057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1962,7 +2067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1972,7 +2077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1982,7 +2087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q39" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1992,7 +2097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2002,7 +2107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q41" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2012,7 +2117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q42" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2022,7 +2127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q43" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2032,7 +2137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q44" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2042,7 +2147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q45" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2052,7 +2157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q46" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2062,7 +2167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q47" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2072,7 +2177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q48" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2082,7 +2187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q49" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2092,7 +2197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q50" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2102,7 +2207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q51" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2112,7 +2217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q52" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2122,7 +2227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q53" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2132,7 +2237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q54" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2142,7 +2247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q55" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2152,7 +2257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q56" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2162,7 +2267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q57" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2172,7 +2277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q58" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2182,7 +2287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q59" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2192,7 +2297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q60" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2202,7 +2307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q61" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2212,7 +2317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q62" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2222,7 +2327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q63" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2232,7 +2337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q64" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2242,7 +2347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q65" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2252,9 +2357,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q66" s="3">
-        <f t="shared" ref="Q66:Q97" si="2">SUM(G66:P66)</f>
+        <f t="shared" ref="Q66:Q80" si="2">SUM(G66:P66)</f>
         <v>0</v>
       </c>
       <c r="S66" s="3">
@@ -2262,7 +2367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q67" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2272,7 +2377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q68" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2282,7 +2387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q69" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2292,7 +2397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q70" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2302,7 +2407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q71" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2312,7 +2417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q72" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2322,7 +2427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q73" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2332,7 +2437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q74" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2342,7 +2447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q75" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2352,7 +2457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q76" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2362,7 +2467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q77" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2372,7 +2477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q78" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2382,7 +2487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q79" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2392,7 +2497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="17:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="17:19" x14ac:dyDescent="0.35">
       <c r="Q80" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2411,21 +2516,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="1" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="1025" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2475,7 +2580,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O2">
         <f t="shared" ref="O2:O33" si="0">SUM(E2:N2)</f>
         <v>0</v>
@@ -2485,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2495,7 +2600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2505,7 +2610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2515,7 +2620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2525,7 +2630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2535,7 +2640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2545,7 +2650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2555,7 +2660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2565,7 +2670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2575,7 +2680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2585,7 +2690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2595,7 +2700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2605,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2615,7 +2720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="O16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2625,7 +2730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2635,7 +2740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2645,7 +2750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2655,7 +2760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2665,7 +2770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2675,7 +2780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2685,7 +2790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2695,7 +2800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2705,7 +2810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O25">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2715,7 +2820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2725,7 +2830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2735,7 +2840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2745,7 +2850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O29">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2755,7 +2860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O30">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2765,7 +2870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O31">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2775,7 +2880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2785,7 +2890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O33">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2795,7 +2900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O34">
         <f t="shared" ref="O34:O65" si="1">SUM(E34:N34)</f>
         <v>0</v>
@@ -2805,7 +2910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2815,7 +2920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O36">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2825,7 +2930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O37">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2835,7 +2940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O38">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2845,7 +2950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2855,7 +2960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O40">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2865,7 +2970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O41">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2875,7 +2980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O42">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2885,7 +2990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O43">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2895,7 +3000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2905,7 +3010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O45">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2915,7 +3020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O46">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2925,7 +3030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O47">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2935,7 +3040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2945,7 +3050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O49">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2955,7 +3060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2965,7 +3070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O51">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2975,7 +3080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O52">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2985,7 +3090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O53">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2995,7 +3100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O54">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3005,7 +3110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O55">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3015,7 +3120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O56">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3025,7 +3130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O57">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3035,7 +3140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O58">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3045,7 +3150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O59">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3055,7 +3160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O60">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3065,7 +3170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O61">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3075,7 +3180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O62">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3085,7 +3190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O63">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3095,7 +3200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O64">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3105,7 +3210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O65">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3115,9 +3220,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O66">
-        <f t="shared" ref="O66:O97" si="2">SUM(E66:N66)</f>
+        <f t="shared" ref="O66:O79" si="2">SUM(E66:N66)</f>
         <v>0</v>
       </c>
       <c r="P66" s="4">
@@ -3125,7 +3230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O67">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3135,7 +3240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O68">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3145,7 +3250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O69">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3155,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O70">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3165,7 +3270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O71">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3175,7 +3280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O72">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3185,7 +3290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O73">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3195,7 +3300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O74">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3205,7 +3310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O75">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3215,7 +3320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O76">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3225,7 +3330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O77">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3235,7 +3340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O78">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3245,7 +3350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O79">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3262,21 +3367,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="1" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="1025" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3299,475 +3404,475 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G2">
         <f t="shared" ref="G2:G33" si="0">(E2+(F2*2))/3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G34">
         <f t="shared" ref="G34:G65" si="1">(E34+(F34*2))/3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G42">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G63">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G64">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G66">
-        <f t="shared" ref="G66:G97" si="2">(E66+(F66*2))/3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G66:G80" si="2">(E66+(F66*2))/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G69">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G71">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G72">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G73">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G74">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G75">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G76">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G78">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G79">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G80">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3781,19 +3886,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1025" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -3811,7 +3916,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3823,7 +3928,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
@@ -3849,7 +3954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -3875,7 +3980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>38</v>
       </c>
@@ -3901,7 +4006,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
@@ -3927,7 +4032,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>42</v>
       </c>
@@ -3953,7 +4058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>43</v>
       </c>
@@ -3979,7 +4084,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>44</v>
       </c>
@@ -4005,7 +4110,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>46</v>
       </c>
@@ -4031,7 +4136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>47</v>
       </c>
@@ -4057,7 +4162,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>49</v>
       </c>
@@ -4083,7 +4188,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>50</v>
       </c>
@@ -4109,7 +4214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>52</v>
       </c>
@@ -4135,7 +4240,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>54</v>
       </c>
@@ -4161,7 +4266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4173,7 +4278,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>100</v>
       </c>
@@ -4193,7 +4298,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>99</v>
       </c>
@@ -4213,7 +4318,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>98</v>
       </c>
@@ -4233,7 +4338,7 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>97</v>
       </c>
@@ -4253,7 +4358,7 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>96</v>
       </c>
@@ -4273,7 +4378,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>95</v>
       </c>
@@ -4293,7 +4398,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>94</v>
       </c>
@@ -4313,7 +4418,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>93</v>
       </c>
@@ -4333,7 +4438,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>92</v>
       </c>
@@ -4353,7 +4458,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>91</v>
       </c>
@@ -4373,7 +4478,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>90</v>
       </c>
@@ -4393,7 +4498,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>89</v>
       </c>
@@ -4413,7 +4518,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>88</v>
       </c>
@@ -4433,7 +4538,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>87</v>
       </c>
@@ -4453,7 +4558,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>86</v>
       </c>
@@ -4473,7 +4578,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>85</v>
       </c>
@@ -4493,7 +4598,7 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>84</v>
       </c>
@@ -4513,7 +4618,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>83</v>
       </c>
@@ -4533,7 +4638,7 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>82</v>
       </c>
@@ -4553,7 +4658,7 @@
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>81</v>
       </c>
@@ -4573,7 +4678,7 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>80</v>
       </c>
@@ -4593,7 +4698,7 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>79</v>
       </c>
@@ -4613,7 +4718,7 @@
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>78</v>
       </c>
@@ -4633,7 +4738,7 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>77</v>
       </c>
@@ -4653,7 +4758,7 @@
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>76</v>
       </c>
@@ -4673,7 +4778,7 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>75</v>
       </c>
@@ -4693,7 +4798,7 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>74</v>
       </c>
@@ -4713,7 +4818,7 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>73</v>
       </c>
@@ -4733,7 +4838,7 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>72</v>
       </c>
@@ -4753,7 +4858,7 @@
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>71</v>
       </c>
@@ -4773,7 +4878,7 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>70</v>
       </c>
@@ -4793,7 +4898,7 @@
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>69</v>
       </c>
@@ -4809,7 +4914,7 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>68</v>
       </c>
@@ -4825,7 +4930,7 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>67</v>
       </c>
@@ -4841,7 +4946,7 @@
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>66</v>
       </c>
@@ -4857,7 +4962,7 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>65</v>
       </c>
@@ -4873,7 +4978,7 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>64</v>
       </c>
@@ -4889,7 +4994,7 @@
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>63</v>
       </c>
@@ -4905,7 +5010,7 @@
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>62</v>
       </c>
@@ -4921,7 +5026,7 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>61</v>
       </c>
@@ -4937,7 +5042,7 @@
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>60</v>
       </c>
@@ -4953,7 +5058,7 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>59</v>
       </c>
@@ -4969,7 +5074,7 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -4985,7 +5090,7 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>57</v>
       </c>
@@ -5001,7 +5106,7 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>56</v>
       </c>
@@ -5017,7 +5122,7 @@
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>55</v>
       </c>
@@ -5033,7 +5138,7 @@
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>54</v>
       </c>
@@ -5049,7 +5154,7 @@
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>53</v>
       </c>
@@ -5065,7 +5170,7 @@
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
         <v>52</v>
       </c>
@@ -5081,7 +5186,7 @@
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>51</v>
       </c>
@@ -5097,7 +5202,7 @@
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>50</v>
       </c>
@@ -5113,7 +5218,7 @@
       <c r="I67" s="6"/>
       <c r="J67" s="6"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>49</v>
       </c>
@@ -5129,7 +5234,7 @@
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
         <v>48</v>
       </c>
@@ -5145,7 +5250,7 @@
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
         <v>47</v>
       </c>
@@ -5161,7 +5266,7 @@
       <c r="I70" s="6"/>
       <c r="J70" s="6"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
         <v>46</v>
       </c>
@@ -5177,7 +5282,7 @@
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
         <v>45</v>
       </c>
@@ -5193,7 +5298,7 @@
       <c r="I72" s="6"/>
       <c r="J72" s="6"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
         <v>44</v>
       </c>
@@ -5209,7 +5314,7 @@
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
         <v>43</v>
       </c>
@@ -5225,7 +5330,7 @@
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
         <v>42</v>
       </c>
@@ -5241,7 +5346,7 @@
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
         <v>41</v>
       </c>
@@ -5257,7 +5362,7 @@
       <c r="I76" s="6"/>
       <c r="J76" s="6"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
         <v>40</v>
       </c>
@@ -5273,7 +5378,7 @@
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
         <v>39</v>
       </c>
@@ -5289,7 +5394,7 @@
       <c r="I78" s="6"/>
       <c r="J78" s="6"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
         <v>38</v>
       </c>
@@ -5305,7 +5410,7 @@
       <c r="I79" s="6"/>
       <c r="J79" s="6"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
         <v>37</v>
       </c>
@@ -5321,7 +5426,7 @@
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
         <v>36</v>
       </c>
@@ -5337,7 +5442,7 @@
       <c r="I81" s="6"/>
       <c r="J81" s="6"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
         <v>35</v>
       </c>
@@ -5353,7 +5458,7 @@
       <c r="I82" s="6"/>
       <c r="J82" s="6"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
         <v>34</v>
       </c>
@@ -5369,7 +5474,7 @@
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
         <v>33</v>
       </c>
@@ -5385,7 +5490,7 @@
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
         <v>32</v>
       </c>
@@ -5401,7 +5506,7 @@
       <c r="I85" s="6"/>
       <c r="J85" s="6"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
         <v>31</v>
       </c>
@@ -5417,7 +5522,7 @@
       <c r="I86" s="6"/>
       <c r="J86" s="6"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
         <v>30</v>
       </c>
@@ -5433,7 +5538,7 @@
       <c r="I87" s="6"/>
       <c r="J87" s="6"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
         <v>29</v>
       </c>
@@ -5449,7 +5554,7 @@
       <c r="I88" s="6"/>
       <c r="J88" s="6"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
         <v>28</v>
       </c>
@@ -5465,7 +5570,7 @@
       <c r="I89" s="6"/>
       <c r="J89" s="6"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
         <v>27</v>
       </c>
@@ -5481,7 +5586,7 @@
       <c r="I90" s="6"/>
       <c r="J90" s="6"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
         <v>26</v>
       </c>
@@ -5497,7 +5602,7 @@
       <c r="I91" s="6"/>
       <c r="J91" s="6"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
         <v>25</v>
       </c>
@@ -5513,7 +5618,7 @@
       <c r="I92" s="6"/>
       <c r="J92" s="6"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
         <v>24</v>
       </c>
@@ -5529,7 +5634,7 @@
       <c r="I93" s="6"/>
       <c r="J93" s="6"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
         <v>23</v>
       </c>
@@ -5545,7 +5650,7 @@
       <c r="I94" s="6"/>
       <c r="J94" s="6"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
         <v>22</v>
       </c>
@@ -5561,7 +5666,7 @@
       <c r="I95" s="6"/>
       <c r="J95" s="6"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
         <v>21</v>
       </c>
@@ -5577,7 +5682,7 @@
       <c r="I96" s="6"/>
       <c r="J96" s="6"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
         <v>20</v>
       </c>
@@ -5593,7 +5698,7 @@
       <c r="I97" s="6"/>
       <c r="J97" s="6"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
         <v>19</v>
       </c>
@@ -5609,7 +5714,7 @@
       <c r="I98" s="6"/>
       <c r="J98" s="6"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
         <v>18</v>
       </c>
@@ -5625,7 +5730,7 @@
       <c r="I99" s="6"/>
       <c r="J99" s="6"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
         <v>17</v>
       </c>
@@ -5641,7 +5746,7 @@
       <c r="I100" s="6"/>
       <c r="J100" s="6"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
         <v>16</v>
       </c>
@@ -5657,7 +5762,7 @@
       <c r="I101" s="6"/>
       <c r="J101" s="6"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
         <v>15</v>
       </c>
@@ -5673,7 +5778,7 @@
       <c r="I102" s="6"/>
       <c r="J102" s="6"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
         <v>14</v>
       </c>
@@ -5689,7 +5794,7 @@
       <c r="I103" s="6"/>
       <c r="J103" s="6"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
         <v>13</v>
       </c>
@@ -5705,7 +5810,7 @@
       <c r="I104" s="6"/>
       <c r="J104" s="6"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
         <v>12</v>
       </c>
@@ -5721,7 +5826,7 @@
       <c r="I105" s="6"/>
       <c r="J105" s="6"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
         <v>11</v>
       </c>
@@ -5737,7 +5842,7 @@
       <c r="I106" s="6"/>
       <c r="J106" s="6"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
         <v>10</v>
       </c>
@@ -5753,7 +5858,7 @@
       <c r="I107" s="6"/>
       <c r="J107" s="6"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
         <v>9</v>
       </c>
@@ -5769,7 +5874,7 @@
       <c r="I108" s="6"/>
       <c r="J108" s="6"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="6">
         <v>8</v>
       </c>
@@ -5785,7 +5890,7 @@
       <c r="I109" s="6"/>
       <c r="J109" s="6"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="6">
         <v>7</v>
       </c>
@@ -5801,7 +5906,7 @@
       <c r="I110" s="6"/>
       <c r="J110" s="6"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="6">
         <v>6</v>
       </c>
@@ -5817,7 +5922,7 @@
       <c r="I111" s="6"/>
       <c r="J111" s="6"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="6">
         <v>5</v>
       </c>
@@ -5833,7 +5938,7 @@
       <c r="I112" s="6"/>
       <c r="J112" s="6"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="6">
         <v>4</v>
       </c>
@@ -5849,7 +5954,7 @@
       <c r="I113" s="6"/>
       <c r="J113" s="6"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="6">
         <v>3</v>
       </c>
@@ -5865,7 +5970,7 @@
       <c r="I114" s="6"/>
       <c r="J114" s="6"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="6">
         <v>2</v>
       </c>
@@ -5881,7 +5986,7 @@
       <c r="I115" s="6"/>
       <c r="J115" s="6"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="6">
         <v>1</v>
       </c>
@@ -5897,7 +6002,7 @@
       <c r="I116" s="6"/>
       <c r="J116" s="6"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="6">
         <v>0</v>
       </c>

</xml_diff>